<commit_message>
Tings are happening hard
</commit_message>
<xml_diff>
--- a/Global_M2/Datasums/Long27_DataComp.xlsx
+++ b/Global_M2/Datasums/Long27_DataComp.xlsx
@@ -506,7 +506,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D2" t="n">
         <v>500</v>
@@ -515,13 +515,13 @@
         <v>35065</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>45413</v>
+        <v>45444</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>30256</v>
+        <v>30319</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -555,10 +555,10 @@
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" s="2" t="n">
-        <v>30225</v>
+        <v>30256</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>45413</v>
+        <v>45444</v>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
@@ -596,16 +596,16 @@
         <v>500</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>30225</v>
+        <v>30256</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>45413</v>
+        <v>45444</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>30256</v>
+        <v>30319</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -641,16 +641,16 @@
         <v>500</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>30225</v>
+        <v>30256</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>45413</v>
+        <v>45444</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>30256</v>
+        <v>30319</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -680,7 +680,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D6" t="n">
         <v>500</v>
@@ -689,13 +689,13 @@
         <v>31747</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>45383</v>
+        <v>45444</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>30256</v>
+        <v>30319</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -731,16 +731,16 @@
         <v>500</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>30195</v>
+        <v>30256</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>45383</v>
+        <v>45444</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>30256</v>
+        <v>30319</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -773,19 +773,19 @@
         <v>500</v>
       </c>
       <c r="D8" t="n">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>30195</v>
+        <v>30256</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>45383</v>
+        <v>45444</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>32813</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -821,16 +821,16 @@
         <v>500</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>30225</v>
+        <v>30256</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>45413</v>
+        <v>45444</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>30256</v>
+        <v>30319</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -863,19 +863,19 @@
         <v>500</v>
       </c>
       <c r="D10" t="n">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>30225</v>
+        <v>30256</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>45413</v>
+        <v>45444</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>30592</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -911,16 +911,16 @@
         <v>500</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>30195</v>
+        <v>30225</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>45383</v>
+        <v>45413</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>30256</v>
+        <v>30319</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -950,22 +950,22 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D12" t="n">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>33939</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>45413</v>
+        <v>45444</v>
       </c>
       <c r="G12" s="2" t="n">
         <v>34578</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -995,7 +995,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="D13" t="n">
         <v>500</v>
@@ -1004,13 +1004,13 @@
         <v>31017</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>45352</v>
+        <v>45413</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>30256</v>
+        <v>30319</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -1043,7 +1043,7 @@
         <v>430</v>
       </c>
       <c r="D14" t="n">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="E14" s="2" t="n">
         <v>32325</v>
@@ -1055,7 +1055,7 @@
         <v>33239</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -1097,10 +1097,10 @@
         <v>45352</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>30225</v>
+        <v>30286</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -1130,22 +1130,22 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D16" t="n">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="E16" s="2" t="n">
         <v>31382</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>45383</v>
+        <v>45413</v>
       </c>
       <c r="G16" s="2" t="n">
         <v>32813</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -1175,22 +1175,22 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="D17" t="n">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>33970</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>45383</v>
+        <v>45444</v>
       </c>
       <c r="G17" s="2" t="n">
         <v>33298</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
@@ -1223,19 +1223,19 @@
         <v>500</v>
       </c>
       <c r="D18" t="n">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>30195</v>
+        <v>30256</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>45383</v>
+        <v>45444</v>
       </c>
       <c r="G18" s="2" t="n">
         <v>37377</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
@@ -1268,19 +1268,19 @@
         <v>500</v>
       </c>
       <c r="D19" t="n">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>30225</v>
+        <v>30256</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>45413</v>
+        <v>45444</v>
       </c>
       <c r="G19" s="2" t="n">
         <v>33178</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
@@ -1310,7 +1310,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="D20" t="n">
         <v>500</v>
@@ -1319,13 +1319,13 @@
         <v>25903</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>45383</v>
+        <v>45444</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>30256</v>
+        <v>30319</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
@@ -1361,16 +1361,16 @@
         <v>500</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>30164</v>
+        <v>30225</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>45352</v>
+        <v>45413</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>30256</v>
+        <v>30319</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
@@ -1403,19 +1403,19 @@
         <v>500</v>
       </c>
       <c r="D22" t="n">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>30195</v>
+        <v>30256</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>45383</v>
+        <v>45444</v>
       </c>
       <c r="G22" s="2" t="n">
         <v>33725</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
@@ -1448,19 +1448,19 @@
         <v>500</v>
       </c>
       <c r="D23" t="n">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>30195</v>
+        <v>30225</v>
       </c>
       <c r="F23" s="2" t="n">
-        <v>45383</v>
+        <v>45413</v>
       </c>
       <c r="G23" s="2" t="n">
         <v>35339</v>
       </c>
       <c r="H23" s="2" t="n">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
@@ -1490,7 +1490,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="D24" t="n">
         <v>500</v>
@@ -1499,13 +1499,13 @@
         <v>33239</v>
       </c>
       <c r="F24" s="2" t="n">
-        <v>45352</v>
+        <v>45444</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>30256</v>
+        <v>30319</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
@@ -1547,10 +1547,10 @@
         <v>45413</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>30256</v>
+        <v>30319</v>
       </c>
       <c r="H25" s="2" t="n">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
@@ -1580,22 +1580,22 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="D26" t="n">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="E26" s="2" t="n">
         <v>31413</v>
       </c>
       <c r="F26" s="2" t="n">
-        <v>45383</v>
+        <v>45444</v>
       </c>
       <c r="G26" s="2" t="n">
         <v>33178</v>
       </c>
       <c r="H26" s="2" t="n">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
@@ -1628,19 +1628,19 @@
         <v>500</v>
       </c>
       <c r="D27" t="n">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>30225</v>
+        <v>30256</v>
       </c>
       <c r="F27" s="2" t="n">
-        <v>45413</v>
+        <v>45444</v>
       </c>
       <c r="G27" s="2" t="n">
         <v>32813</v>
       </c>
       <c r="H27" s="2" t="n">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
@@ -1670,22 +1670,22 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="D28" t="n">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="E28" s="2" t="n">
         <v>34304</v>
       </c>
       <c r="F28" s="2" t="n">
-        <v>45383</v>
+        <v>45444</v>
       </c>
       <c r="G28" s="2" t="n">
         <v>34121</v>
       </c>
       <c r="H28" s="2" t="n">
-        <v>45446</v>
+        <v>45505</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>

</xml_diff>